<commit_message>
chore: update Excel training files with latest changes
</commit_message>
<xml_diff>
--- a/Excel_PowerBI/EXCEL_DAY_2.xlsx
+++ b/Excel_PowerBI/EXCEL_DAY_2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Documents\Projects\Pyspiders\Excel_PowerBI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35018751-8AC4-4A02-8C77-416AFB35ADF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECF6A6D-BFAF-4B66-8367-193B443D0853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D57CBD8D-DD7B-4CB4-A2DF-05F7A1811C2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>SID</t>
   </si>
@@ -243,7 +244,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="213">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -365,6 +376,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -454,6 +505,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -553,6 +634,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -642,6 +763,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -721,6 +892,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="0.39994506668294322"/>
       </font>
       <border>
@@ -730,6 +921,1174 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1000,6 +2359,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1100,64 +2464,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1169,64 +2533,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,64 +2631,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1336,64 +2700,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,64 +2798,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1503,64 +2867,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>50</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>78</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>76</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>99</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,64 +2965,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1670,64 +3034,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,64 +3132,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1837,64 +3201,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>98</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1935,64 +3299,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Naveen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yaseen</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sanjay</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Rohith</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Dharshan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Veerash</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ahmadh</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Hari</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Soma</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Gopi</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Praveen</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Rashad</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sunil</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Dhanush</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Vijay</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Goplan</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>RAM</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Yaseen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Ahmadh</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
+                  <c:v>Ajith</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Pramith</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Mohammed</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Rashad</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gopi</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Dhanush</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Dharshan</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Vijay</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sunil</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Ajith</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Sanjay</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Hari</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Goplan</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Veerash</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Soma</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Naveen</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Praveen</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Pramith</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2004,64 +3368,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2817,14 +4181,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
@@ -3151,10 +4515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D74232-DF13-4896-9C34-D08DC8A6C17F}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="H2" sqref="H2:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3163,7 +4527,7 @@
     <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3191,635 +4555,832 @@
       <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" s="6">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="6">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F2" s="6">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="G2" s="6">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="H2" s="6">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="I2" s="7">
         <v>45076</v>
       </c>
+      <c r="L2" s="6">
+        <v>78</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="6">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="D3" s="6">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6">
         <v>26</v>
       </c>
-      <c r="E3" s="6">
-        <v>91</v>
-      </c>
       <c r="F3" s="6">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H3" s="6">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I3" s="7">
         <v>45076</v>
       </c>
+      <c r="L3" s="6">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="6">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E4" s="6">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F4" s="6">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G4" s="6">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="H4" s="6">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="I4" s="7">
         <v>45076</v>
       </c>
+      <c r="L4" s="6">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="D5" s="6">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E5" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F5" s="6">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H5" s="6">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I5" s="7">
         <v>45076</v>
       </c>
+      <c r="L5" s="6">
+        <v>74</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E6" s="6">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F6" s="6">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G6" s="6">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="H6" s="6">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="I6" s="7">
         <v>45076</v>
       </c>
+      <c r="L6" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D7" s="6">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E7" s="6">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F7" s="6">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G7" s="6">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="H7" s="6">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="I7" s="7">
         <v>45076</v>
       </c>
+      <c r="L7" s="6">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="6">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F8" s="6">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G8" s="6">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="H8" s="6">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I8" s="7">
         <v>45076</v>
       </c>
+      <c r="L8" s="6">
+        <v>65</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6">
+        <v>98</v>
+      </c>
+      <c r="D9" s="6">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6">
+        <v>41</v>
+      </c>
+      <c r="G9" s="6">
         <v>89</v>
       </c>
-      <c r="D9" s="6">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="H9" s="6">
+        <v>63</v>
+      </c>
+      <c r="I9" s="7">
+        <v>45838</v>
+      </c>
+      <c r="L9" s="6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45</v>
+      </c>
+      <c r="E10" s="6">
         <v>78</v>
       </c>
-      <c r="F9" s="6">
-        <v>93</v>
-      </c>
-      <c r="G9" s="6">
-        <v>21</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="F10" s="6">
+        <v>53</v>
+      </c>
+      <c r="G10" s="6">
         <v>57</v>
       </c>
-      <c r="I9" s="7">
-        <v>45076</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6">
-        <v>55</v>
-      </c>
-      <c r="E10" s="6">
-        <v>14</v>
-      </c>
-      <c r="F10" s="6">
-        <v>84</v>
-      </c>
-      <c r="G10" s="6">
-        <v>10</v>
-      </c>
       <c r="H10" s="6">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I10" s="7">
         <v>45076</v>
       </c>
+      <c r="L10" s="6">
+        <v>77</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6">
         <v>17</v>
       </c>
-      <c r="C11" s="6">
-        <v>49</v>
-      </c>
-      <c r="D11" s="6">
-        <v>92</v>
-      </c>
       <c r="E11" s="6">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="F11" s="6">
+        <v>70</v>
+      </c>
+      <c r="G11" s="6">
+        <v>51</v>
+      </c>
+      <c r="H11" s="6">
         <v>65</v>
-      </c>
-      <c r="G11" s="6">
-        <v>46</v>
-      </c>
-      <c r="H11" s="6">
-        <v>53</v>
       </c>
       <c r="I11" s="7">
         <v>45076</v>
       </c>
+      <c r="L11" s="6">
+        <v>53</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D12" s="6">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="E12" s="6">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="F12" s="6">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G12" s="6">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H12" s="6">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I12" s="7">
         <v>45076</v>
       </c>
+      <c r="L12" s="6">
+        <v>63</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="6">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="E13" s="6">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="F13" s="6">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="G13" s="6">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H13" s="6">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="I13" s="7">
         <v>45076</v>
       </c>
+      <c r="L13" s="6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D14" s="6">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="E14" s="6">
         <v>43</v>
       </c>
       <c r="F14" s="6">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="G14" s="6">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H14" s="6">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="I14" s="7">
         <v>45076</v>
       </c>
+      <c r="L14" s="6">
+        <v>84</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6">
+        <v>89</v>
+      </c>
+      <c r="D15" s="6">
+        <v>38</v>
+      </c>
+      <c r="E15" s="6">
+        <v>78</v>
+      </c>
+      <c r="F15" s="6">
+        <v>93</v>
+      </c>
+      <c r="G15" s="6">
         <v>21</v>
       </c>
-      <c r="C15" s="6">
-        <v>98</v>
-      </c>
-      <c r="D15" s="6">
-        <v>24</v>
-      </c>
-      <c r="E15" s="6">
-        <v>25</v>
-      </c>
-      <c r="F15" s="6">
-        <v>41</v>
-      </c>
-      <c r="G15" s="6">
-        <v>89</v>
-      </c>
       <c r="H15" s="6">
+        <v>74</v>
+      </c>
+      <c r="I15" s="7">
+        <v>45076</v>
+      </c>
+      <c r="L15" s="6">
         <v>73</v>
       </c>
-      <c r="I15" s="7">
-        <v>45838</v>
-      </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16" s="6">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="D16" s="6">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E16" s="6">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F16" s="6">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G16" s="6">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="H16" s="6">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="I16" s="7">
         <v>45076</v>
       </c>
+      <c r="L16" s="6">
+        <v>44</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="6">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D17" s="6">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="6">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="F17" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G17" s="6">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H17" s="6">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I17" s="7">
         <v>45076</v>
       </c>
+      <c r="L17" s="6">
+        <v>75</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D18" s="6">
+        <v>26</v>
+      </c>
+      <c r="E18" s="6">
+        <v>91</v>
+      </c>
+      <c r="F18" s="6">
         <v>45</v>
       </c>
-      <c r="E18" s="6">
+      <c r="G18" s="6">
+        <v>22</v>
+      </c>
+      <c r="H18" s="6">
         <v>78</v>
-      </c>
-      <c r="F18" s="6">
-        <v>53</v>
-      </c>
-      <c r="G18" s="6">
-        <v>57</v>
-      </c>
-      <c r="H18" s="6">
-        <v>66</v>
       </c>
       <c r="I18" s="7">
         <v>45076</v>
       </c>
+      <c r="L18" s="6">
+        <v>66</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="6">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="D19" s="6">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="E19" s="6">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="F19" s="6">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G19" s="6">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H19" s="6">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="I19" s="7">
         <v>45076</v>
       </c>
+      <c r="L19" s="6">
+        <v>99</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="6">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D20" s="6">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E20" s="6">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="F20" s="6">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="G20" s="6">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="H20" s="6">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="I20" s="7">
         <v>45076</v>
       </c>
+      <c r="L20" s="6">
+        <v>65</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="6">
+        <v>74</v>
+      </c>
+      <c r="D21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="6">
-        <v>38</v>
-      </c>
-      <c r="D21" s="6">
-        <v>39</v>
-      </c>
       <c r="E21" s="6">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6">
+        <v>96</v>
+      </c>
+      <c r="G21" s="6">
+        <v>66</v>
+      </c>
+      <c r="H21" s="6">
         <v>99</v>
-      </c>
-      <c r="F21" s="6">
-        <v>11</v>
-      </c>
-      <c r="G21" s="6">
-        <v>64</v>
-      </c>
-      <c r="H21" s="6">
-        <v>30</v>
       </c>
       <c r="I21" s="7">
         <v>45076</v>
       </c>
+      <c r="L21" s="6">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:H21">
+    <sortCondition ref="H1:H21"/>
+  </sortState>
   <conditionalFormatting sqref="C2:C21">
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
       <formula>75</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="lessThan">
       <formula>35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="between">
       <formula>35</formula>
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D21 F2:H21">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
       <formula>35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
       <formula>35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="between">
       <formula>35</formula>
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D21 F2:H21">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="as">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="as">
       <formula>NOT(ISERROR(SEARCH("as",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I21">
-    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="16" priority="17" timePeriod="yesterday">
       <formula>FLOOR(I2,1)=TODAY()-1</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="15" priority="16" timePeriod="lastMonth">
       <formula>AND(MONTH(I2)=MONTH(EDATE(TODAY(),0-1)),YEAR(I2)=YEAR(EDATE(TODAY(),0-1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:H21">
+    <cfRule type="top10" dxfId="14" priority="15" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="14" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22:L1048576 L1">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E0967AEE-795C-49B5-B231-8BE3031E9DBE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L21">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0A23B07B-67CB-40D8-A469-15EB5763A42F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H21">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{70938D27-7B49-4455-99E2-C2387FF42E57}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E0967AEE-795C-49B5-B231-8BE3031E9DBE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L22:L1048576 L1</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0A23B07B-67CB-40D8-A469-15EB5763A42F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L2:L21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{70938D27-7B49-4455-99E2-C2387FF42E57}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H21</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0666AF1-1EBD-45C0-9A5F-6907AB79A5F2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>